<commit_message>
Aggiunto punteggio medio al foglio di calcolo SUS
</commit_message>
<xml_diff>
--- a/Questionari/SUS/SUS-Foglio di calcolo.xlsx
+++ b/Questionari/SUS/SUS-Foglio di calcolo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\IUM progetto\Progetto-IUM-21-22\Questionari\SUS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuse\Desktop\Importanti\Università\3° Anno\IUM\Progetto IUM 21-22\Questionari\SUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7527EAC8-DD8F-4353-99DB-160A442F43DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDB0946-ABF9-4251-8C85-1676A2BE6FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="5910" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <r>
       <rPr>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Partecipante n.4</t>
+  </si>
+  <si>
+    <t>Punteggio medio</t>
   </si>
 </sst>
 </file>
@@ -230,6 +233,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -237,9 +243,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -557,42 +560,46 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -617,8 +624,9 @@
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="38.25">
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="39.6">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -654,7 +662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:11" ht="26.4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -690,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5">
+    <row r="5" spans="1:11" ht="26.4">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -726,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="38.25">
+    <row r="6" spans="1:11" ht="39.6">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -762,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="38.25">
+    <row r="7" spans="1:11" ht="26.4">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -798,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.5">
+    <row r="8" spans="1:11" ht="26.4">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -834,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:11" ht="52.8">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -870,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5">
+    <row r="10" spans="1:11" ht="26.4">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -906,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.5">
+    <row r="11" spans="1:11" ht="26.4">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -942,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="51">
+    <row r="12" spans="1:11" ht="52.8">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -978,7 +986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="27" customHeight="1">
+    <row r="13" spans="1:11" ht="27" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>15</v>
@@ -993,21 +1001,26 @@
         <f>SUM(F3:F12)*2.5</f>
         <v>47.5</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14">
+      <c r="G13" s="10"/>
+      <c r="H13" s="11">
         <f>SUM(H3:H12)*2.5</f>
         <v>27.5</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14">
+      <c r="I13" s="10"/>
+      <c r="J13" s="11">
         <f>SUM(J3:J12)*2.5</f>
         <v>50</v>
       </c>
+      <c r="K13">
+        <f>AVERAGE(D13,F13,H13,J13)</f>
+        <v>44.375</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>